<commit_message>
Demonstrações e Laboratório até o dia 08/09
</commit_message>
<xml_diff>
--- a/Apoio/Permissoes.xlsx
+++ b/Apoio/Permissoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vithor\source\repos\TREINAMENTO_SSAS\TREINAMENTO_SSAS\Apoio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA176D7-983A-40A5-9DA4-C2CC9D8357BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A4FB68-C6DD-4705-9C83-99E01EB6418C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="4890" windowWidth="21600" windowHeight="11505" xr2:uid="{757126EA-F5BC-4EB6-9855-2D2579CD7ABB}"/>
+    <workbookView xWindow="5010" yWindow="705" windowWidth="21600" windowHeight="11505" xr2:uid="{757126EA-F5BC-4EB6-9855-2D2579CD7ABB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>